<commit_message>
small commit. testing office firewall
</commit_message>
<xml_diff>
--- a/config/emissions_to_energy_mappings.xlsx
+++ b/config/emissions_to_energy_mappings.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="154" documentId="13_ncr:1_{2EC4C934-4881-4B50-B407-0AD672430172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{955330BC-B0C5-4338-AE24-FE76D59EFF8C}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="6420" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="6420" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MAP_Hugh" sheetId="13" r:id="rId1"/>
@@ -981,7 +981,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1625,7 +1625,7 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
     <col min="2" max="2" width="35.7109375" style="6" customWidth="1"/>
@@ -1639,7 +1639,7 @@
     <col min="13" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="B1" s="3" t="s">
         <v>54</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="5" customFormat="1">
       <c r="A2" s="5" t="s">
         <v>87</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" s="4" t="s">
         <v>57</v>
       </c>
@@ -1680,7 +1680,7 @@
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
         <v>57</v>
       </c>
@@ -1690,7 +1690,7 @@
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" s="4" t="s">
         <v>57</v>
       </c>
@@ -1706,7 +1706,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="A6" s="4" t="s">
         <v>57</v>
       </c>
@@ -1722,7 +1722,7 @@
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>57</v>
       </c>
@@ -1738,7 +1738,7 @@
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8">
       <c r="A8" s="4" t="s">
         <v>57</v>
       </c>
@@ -1751,7 +1751,7 @@
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8">
       <c r="A9" s="4" t="s">
         <v>57</v>
       </c>
@@ -1767,7 +1767,7 @@
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="A10" s="4" t="s">
         <v>57</v>
       </c>
@@ -1783,7 +1783,7 @@
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="A11" s="4" t="s">
         <v>57</v>
       </c>
@@ -1796,7 +1796,7 @@
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8">
       <c r="A12" s="4" t="s">
         <v>57</v>
       </c>
@@ -1812,7 +1812,7 @@
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8">
       <c r="A13" s="4" t="s">
         <v>57</v>
       </c>
@@ -1828,7 +1828,7 @@
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8">
       <c r="A14" s="4" t="s">
         <v>57</v>
       </c>
@@ -1844,7 +1844,7 @@
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8">
       <c r="A15" s="4" t="s">
         <v>57</v>
       </c>
@@ -1860,7 +1860,7 @@
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8">
       <c r="A16" s="4" t="s">
         <v>57</v>
       </c>
@@ -1876,7 +1876,7 @@
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9">
       <c r="A17" s="4" t="s">
         <v>57</v>
       </c>
@@ -1889,7 +1889,7 @@
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9">
       <c r="A18" s="4" t="s">
         <v>57</v>
       </c>
@@ -1903,7 +1903,7 @@
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9">
       <c r="A19" s="4" t="s">
         <v>57</v>
       </c>
@@ -1917,7 +1917,7 @@
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9">
       <c r="A20" s="4" t="s">
         <v>57</v>
       </c>
@@ -1930,7 +1930,7 @@
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
     </row>
-    <row r="21" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="17.25">
       <c r="A21" s="4" t="s">
         <v>57</v>
       </c>
@@ -1946,7 +1946,7 @@
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9">
       <c r="A22" s="4" t="s">
         <v>57</v>
       </c>
@@ -1959,7 +1959,7 @@
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9">
       <c r="A23" s="4" t="s">
         <v>57</v>
       </c>
@@ -1972,7 +1972,7 @@
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9">
       <c r="A24" s="4" t="s">
         <v>57</v>
       </c>
@@ -1985,7 +1985,7 @@
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9">
       <c r="A25" s="4" t="s">
         <v>57</v>
       </c>
@@ -1998,7 +1998,7 @@
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9">
       <c r="A26" s="4" t="s">
         <v>57</v>
       </c>
@@ -2014,7 +2014,7 @@
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9">
       <c r="A27" s="4" t="s">
         <v>57</v>
       </c>
@@ -2027,7 +2027,7 @@
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9">
       <c r="A28" s="4" t="s">
         <v>57</v>
       </c>
@@ -2040,7 +2040,7 @@
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9">
       <c r="A29" s="4" t="s">
         <v>57</v>
       </c>
@@ -2056,7 +2056,7 @@
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9">
       <c r="A30" s="4" t="s">
         <v>57</v>
       </c>
@@ -2069,7 +2069,7 @@
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9">
       <c r="A31" s="4" t="s">
         <v>57</v>
       </c>
@@ -2082,7 +2082,7 @@
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9">
       <c r="A32" s="4" t="s">
         <v>57</v>
       </c>
@@ -2095,7 +2095,7 @@
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8">
       <c r="A33" s="4" t="s">
         <v>57</v>
       </c>
@@ -2108,7 +2108,7 @@
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8">
       <c r="A34" s="4" t="s">
         <v>57</v>
       </c>
@@ -2118,7 +2118,7 @@
       <c r="G34" s="10"/>
       <c r="H34" s="11"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8">
       <c r="A35" s="4" t="s">
         <v>57</v>
       </c>
@@ -2134,7 +2134,7 @@
       <c r="G35" s="10"/>
       <c r="H35" s="10"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8">
       <c r="A36" s="4" t="s">
         <v>57</v>
       </c>
@@ -2147,7 +2147,7 @@
       <c r="G36" s="10"/>
       <c r="H36" s="10"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8">
       <c r="A37" s="4" t="s">
         <v>57</v>
       </c>
@@ -2160,7 +2160,7 @@
       <c r="G37" s="10"/>
       <c r="H37" s="10"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8">
       <c r="A38" s="4" t="s">
         <v>57</v>
       </c>
@@ -2173,7 +2173,7 @@
       <c r="G38" s="10"/>
       <c r="H38" s="10"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8">
       <c r="A39" s="4" t="s">
         <v>57</v>
       </c>
@@ -2186,7 +2186,7 @@
       <c r="G39" s="10"/>
       <c r="H39" s="10"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8">
       <c r="A40" s="4" t="s">
         <v>57</v>
       </c>
@@ -2202,7 +2202,7 @@
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
     </row>
-    <row r="41" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="33">
       <c r="A41" s="4" t="s">
         <v>57</v>
       </c>
@@ -2218,7 +2218,7 @@
       <c r="G41" s="10"/>
       <c r="H41" s="10"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8">
       <c r="A42" s="4" t="s">
         <v>57</v>
       </c>
@@ -2234,7 +2234,7 @@
       <c r="G42" s="10"/>
       <c r="H42" s="10"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8">
       <c r="A43" s="4" t="s">
         <v>57</v>
       </c>
@@ -2244,7 +2244,7 @@
       <c r="G43" s="10"/>
       <c r="H43" s="11"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8">
       <c r="A44" s="4" t="s">
         <v>57</v>
       </c>
@@ -2257,7 +2257,7 @@
       <c r="G44" s="10"/>
       <c r="H44" s="10"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8">
       <c r="A45" s="4" t="s">
         <v>76</v>
       </c>
@@ -2273,7 +2273,7 @@
       <c r="G45" s="10"/>
       <c r="H45" s="10"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8">
       <c r="A46" s="4" t="s">
         <v>76</v>
       </c>
@@ -2289,7 +2289,7 @@
       <c r="G46" s="10"/>
       <c r="H46" s="10"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8">
       <c r="A47" s="4" t="s">
         <v>76</v>
       </c>
@@ -2305,7 +2305,7 @@
       <c r="G47" s="10"/>
       <c r="H47" s="10"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8">
       <c r="A48" s="4" t="s">
         <v>76</v>
       </c>
@@ -2321,7 +2321,7 @@
       <c r="G48" s="10"/>
       <c r="H48" s="10"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8">
       <c r="A49" s="4" t="s">
         <v>76</v>
       </c>
@@ -2337,7 +2337,7 @@
       <c r="G49" s="10"/>
       <c r="H49" s="10"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8">
       <c r="A50" s="4" t="s">
         <v>76</v>
       </c>
@@ -2353,7 +2353,7 @@
       <c r="G50" s="10"/>
       <c r="H50" s="10"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8">
       <c r="A51" s="4" t="s">
         <v>76</v>
       </c>
@@ -2369,7 +2369,7 @@
       <c r="G51" s="10"/>
       <c r="H51" s="10"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8">
       <c r="A52" s="4" t="s">
         <v>76</v>
       </c>
@@ -2385,7 +2385,7 @@
       <c r="G52" s="10"/>
       <c r="H52" s="10"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8">
       <c r="A53" s="4" t="s">
         <v>76</v>
       </c>
@@ -2395,7 +2395,7 @@
       <c r="G53" s="10"/>
       <c r="H53" s="10"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8">
       <c r="A54" s="4" t="s">
         <v>76</v>
       </c>
@@ -2405,7 +2405,7 @@
       <c r="G54" s="13"/>
       <c r="H54" s="10"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8">
       <c r="A55" s="4" t="s">
         <v>76</v>
       </c>
@@ -2418,7 +2418,7 @@
       <c r="G55" s="13"/>
       <c r="H55" s="10"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8">
       <c r="A56" s="4" t="s">
         <v>57</v>
       </c>
@@ -2431,7 +2431,7 @@
       <c r="G56" s="13"/>
       <c r="H56" s="10"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8">
       <c r="A57" s="4" t="s">
         <v>57</v>
       </c>
@@ -2445,7 +2445,7 @@
       <c r="G57" s="13"/>
       <c r="H57" s="10"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8">
       <c r="A58" s="4" t="s">
         <v>57</v>
       </c>
@@ -2459,7 +2459,7 @@
       <c r="G58" s="13"/>
       <c r="H58" s="10"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8">
       <c r="A59" s="4" t="s">
         <v>57</v>
       </c>
@@ -2473,121 +2473,121 @@
       <c r="G59" s="13"/>
       <c r="H59" s="12"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8">
       <c r="D60"/>
       <c r="G60" s="13"/>
       <c r="H60" s="10"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8">
       <c r="D61"/>
       <c r="G61" s="13"/>
       <c r="H61" s="10"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8">
       <c r="G62" s="13"/>
       <c r="H62" s="12"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8">
       <c r="G63" s="13"/>
       <c r="H63" s="10"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8">
       <c r="G64" s="13"/>
       <c r="H64" s="10"/>
     </row>
-    <row r="65" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="7:8">
       <c r="G65" s="13"/>
       <c r="H65" s="10"/>
     </row>
-    <row r="66" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="7:8">
       <c r="G66" s="13"/>
       <c r="H66" s="10"/>
     </row>
-    <row r="67" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="7:8">
       <c r="G67" s="13"/>
       <c r="H67" s="10"/>
     </row>
-    <row r="68" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="7:8">
       <c r="G68" s="13"/>
       <c r="H68" s="10"/>
     </row>
-    <row r="69" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="7:8">
       <c r="G69" s="13"/>
       <c r="H69" s="10"/>
     </row>
-    <row r="70" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="7:8">
       <c r="G70" s="13"/>
       <c r="H70" s="10"/>
     </row>
-    <row r="71" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="7:8">
       <c r="G71" s="10"/>
       <c r="H71" s="10"/>
     </row>
-    <row r="72" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="7:8">
       <c r="G72" s="10"/>
       <c r="H72" s="10"/>
     </row>
-    <row r="73" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="7:8">
       <c r="G73" s="10"/>
       <c r="H73" s="10"/>
     </row>
-    <row r="74" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="7:8">
       <c r="G74" s="10"/>
       <c r="H74" s="10"/>
     </row>
-    <row r="75" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="7:8">
       <c r="G75" s="10"/>
       <c r="H75" s="10"/>
     </row>
-    <row r="76" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="7:8">
       <c r="G76" s="10"/>
       <c r="H76" s="10"/>
     </row>
-    <row r="77" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="7:8">
       <c r="G77" s="10"/>
       <c r="H77" s="10"/>
     </row>
-    <row r="78" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="7:8">
       <c r="G78" s="10"/>
       <c r="H78" s="10"/>
     </row>
-    <row r="79" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="7:8">
       <c r="G79" s="10"/>
       <c r="H79" s="10"/>
     </row>
-    <row r="80" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="7:8">
       <c r="G80" s="10"/>
       <c r="H80" s="10"/>
     </row>
-    <row r="81" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="7:8">
       <c r="G81" s="10"/>
       <c r="H81" s="10"/>
     </row>
-    <row r="82" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="7:8">
       <c r="G82" s="10"/>
       <c r="H82" s="10"/>
     </row>
-    <row r="83" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="7:8">
       <c r="G83" s="10"/>
       <c r="H83" s="11"/>
     </row>
-    <row r="84" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="7:8">
       <c r="G84" s="10"/>
       <c r="H84" s="10"/>
     </row>
-    <row r="85" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="7:8">
       <c r="G85" s="10"/>
       <c r="H85" s="10"/>
     </row>
-    <row r="86" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="7:8">
       <c r="G86" s="10"/>
       <c r="H86" s="10"/>
     </row>
-    <row r="87" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="7:8">
       <c r="G87" s="10"/>
       <c r="H87" s="10"/>
     </row>
-    <row r="88" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="7:8">
       <c r="G88" s="10"/>
       <c r="H88" s="10"/>
     </row>
@@ -2601,11 +2601,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A919A1-E034-4E6D-8034-EB37F251255F}">
   <dimension ref="A1:L88"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
     <col min="2" max="2" width="35.7109375" style="6" customWidth="1"/>
@@ -2617,7 +2617,7 @@
     <col min="13" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="B1" s="3" t="s">
         <v>54</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="5" customFormat="1">
       <c r="A2" s="5" t="s">
         <v>87</v>
       </c>
@@ -2637,7 +2637,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" s="4" t="s">
         <v>57</v>
       </c>
@@ -2650,7 +2650,7 @@
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
         <v>57</v>
       </c>
@@ -2661,7 +2661,7 @@
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" s="4" t="s">
         <v>57</v>
       </c>
@@ -2674,7 +2674,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="A6" s="4" t="s">
         <v>57</v>
       </c>
@@ -2687,7 +2687,7 @@
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>57</v>
       </c>
@@ -2700,7 +2700,7 @@
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8">
       <c r="A8" s="4" t="s">
         <v>57</v>
       </c>
@@ -2711,7 +2711,7 @@
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8">
       <c r="A9" s="4" t="s">
         <v>57</v>
       </c>
@@ -2724,7 +2724,7 @@
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="A10" s="4" t="s">
         <v>57</v>
       </c>
@@ -2737,7 +2737,7 @@
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="A11" s="4" t="s">
         <v>57</v>
       </c>
@@ -2748,7 +2748,7 @@
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8">
       <c r="A12" s="4" t="s">
         <v>57</v>
       </c>
@@ -2761,7 +2761,7 @@
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8">
       <c r="A13" s="4" t="s">
         <v>57</v>
       </c>
@@ -2774,7 +2774,7 @@
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8">
       <c r="A14" s="4" t="s">
         <v>57</v>
       </c>
@@ -2787,7 +2787,7 @@
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8">
       <c r="A15" s="4" t="s">
         <v>57</v>
       </c>
@@ -2800,7 +2800,7 @@
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8">
       <c r="A16" s="4" t="s">
         <v>57</v>
       </c>
@@ -2813,7 +2813,7 @@
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8">
       <c r="A17" s="4" t="s">
         <v>57</v>
       </c>
@@ -2824,7 +2824,7 @@
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8">
       <c r="A18" s="4" t="s">
         <v>57</v>
       </c>
@@ -2835,7 +2835,7 @@
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8">
       <c r="A19" s="4" t="s">
         <v>57</v>
       </c>
@@ -2848,7 +2848,7 @@
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8">
       <c r="A20" s="4" t="s">
         <v>57</v>
       </c>
@@ -2861,7 +2861,7 @@
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
     </row>
-    <row r="21" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="17.25">
       <c r="A21" s="4" t="s">
         <v>57</v>
       </c>
@@ -2874,7 +2874,7 @@
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8">
       <c r="A22" s="4" t="s">
         <v>57</v>
       </c>
@@ -2885,7 +2885,7 @@
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8">
       <c r="A23" s="4" t="s">
         <v>57</v>
       </c>
@@ -2896,7 +2896,7 @@
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8">
       <c r="A24" s="4" t="s">
         <v>57</v>
       </c>
@@ -2907,7 +2907,7 @@
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8">
       <c r="A25" s="4" t="s">
         <v>57</v>
       </c>
@@ -2918,7 +2918,7 @@
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8">
       <c r="A26" s="4" t="s">
         <v>57</v>
       </c>
@@ -2931,7 +2931,7 @@
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8">
       <c r="A27" s="4" t="s">
         <v>57</v>
       </c>
@@ -2942,7 +2942,7 @@
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8">
       <c r="A28" s="4" t="s">
         <v>57</v>
       </c>
@@ -2953,7 +2953,7 @@
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8">
       <c r="A29" s="4" t="s">
         <v>57</v>
       </c>
@@ -2966,7 +2966,7 @@
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8">
       <c r="A30" s="4" t="s">
         <v>57</v>
       </c>
@@ -2977,7 +2977,7 @@
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8">
       <c r="A31" s="4" t="s">
         <v>57</v>
       </c>
@@ -2988,7 +2988,7 @@
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8">
       <c r="A32" s="4" t="s">
         <v>57</v>
       </c>
@@ -2999,7 +2999,7 @@
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8">
       <c r="A33" s="4" t="s">
         <v>57</v>
       </c>
@@ -3010,7 +3010,7 @@
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8">
       <c r="A34" s="4" t="s">
         <v>57</v>
       </c>
@@ -3021,7 +3021,7 @@
       <c r="G34" s="10"/>
       <c r="H34" s="11"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8">
       <c r="A35" s="4" t="s">
         <v>57</v>
       </c>
@@ -3034,7 +3034,7 @@
       <c r="G35" s="10"/>
       <c r="H35" s="10"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8">
       <c r="A36" s="4" t="s">
         <v>57</v>
       </c>
@@ -3045,7 +3045,7 @@
       <c r="G36" s="10"/>
       <c r="H36" s="10"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8">
       <c r="A37" s="4" t="s">
         <v>57</v>
       </c>
@@ -3056,7 +3056,7 @@
       <c r="G37" s="10"/>
       <c r="H37" s="10"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8">
       <c r="A38" s="4" t="s">
         <v>57</v>
       </c>
@@ -3067,7 +3067,7 @@
       <c r="G38" s="10"/>
       <c r="H38" s="10"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8">
       <c r="A39" s="4" t="s">
         <v>57</v>
       </c>
@@ -3078,7 +3078,7 @@
       <c r="G39" s="10"/>
       <c r="H39" s="10"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8">
       <c r="A40" s="4" t="s">
         <v>57</v>
       </c>
@@ -3091,7 +3091,7 @@
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
     </row>
-    <row r="41" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="33">
       <c r="A41" s="4" t="s">
         <v>57</v>
       </c>
@@ -3104,7 +3104,7 @@
       <c r="G41" s="10"/>
       <c r="H41" s="10"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8">
       <c r="A42" s="4" t="s">
         <v>57</v>
       </c>
@@ -3117,7 +3117,7 @@
       <c r="G42" s="10"/>
       <c r="H42" s="10"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8">
       <c r="A43" s="4" t="s">
         <v>57</v>
       </c>
@@ -3128,7 +3128,7 @@
       <c r="G43" s="10"/>
       <c r="H43" s="11"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8">
       <c r="A44" s="4" t="s">
         <v>57</v>
       </c>
@@ -3139,7 +3139,7 @@
       <c r="G44" s="10"/>
       <c r="H44" s="10"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8">
       <c r="A45" s="4" t="s">
         <v>76</v>
       </c>
@@ -3152,7 +3152,7 @@
       <c r="G45" s="10"/>
       <c r="H45" s="10"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8">
       <c r="A46" s="4" t="s">
         <v>76</v>
       </c>
@@ -3165,7 +3165,7 @@
       <c r="G46" s="10"/>
       <c r="H46" s="10"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8">
       <c r="A47" s="4" t="s">
         <v>76</v>
       </c>
@@ -3178,7 +3178,7 @@
       <c r="G47" s="10"/>
       <c r="H47" s="10"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8">
       <c r="A48" s="4" t="s">
         <v>76</v>
       </c>
@@ -3191,7 +3191,7 @@
       <c r="G48" s="10"/>
       <c r="H48" s="10"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8">
       <c r="A49" s="4" t="s">
         <v>76</v>
       </c>
@@ -3204,7 +3204,7 @@
       <c r="G49" s="10"/>
       <c r="H49" s="10"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8">
       <c r="A50" s="4" t="s">
         <v>76</v>
       </c>
@@ -3217,7 +3217,7 @@
       <c r="G50" s="10"/>
       <c r="H50" s="10"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8">
       <c r="A51" s="4" t="s">
         <v>76</v>
       </c>
@@ -3230,7 +3230,7 @@
       <c r="G51" s="10"/>
       <c r="H51" s="10"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8">
       <c r="A52" s="4" t="s">
         <v>76</v>
       </c>
@@ -3243,7 +3243,7 @@
       <c r="G52" s="10"/>
       <c r="H52" s="10"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8">
       <c r="A53" s="4" t="s">
         <v>76</v>
       </c>
@@ -3254,7 +3254,7 @@
       <c r="G53" s="10"/>
       <c r="H53" s="10"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8">
       <c r="A54" s="4" t="s">
         <v>76</v>
       </c>
@@ -3265,7 +3265,7 @@
       <c r="G54" s="10"/>
       <c r="H54" s="10"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8">
       <c r="A55" s="4" t="s">
         <v>76</v>
       </c>
@@ -3278,142 +3278,142 @@
       <c r="G55" s="10"/>
       <c r="H55" s="10"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8">
       <c r="G56" s="10"/>
       <c r="H56" s="10"/>
     </row>
-    <row r="57" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="15">
       <c r="B57" s="8"/>
       <c r="C57"/>
       <c r="G57" s="10"/>
       <c r="H57" s="10"/>
     </row>
-    <row r="58" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="15">
       <c r="B58" s="8"/>
       <c r="C58"/>
       <c r="G58" s="10"/>
       <c r="H58" s="10"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8">
       <c r="C59"/>
       <c r="G59" s="10"/>
       <c r="H59" s="12"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8">
       <c r="C60"/>
       <c r="G60" s="10"/>
       <c r="H60" s="10"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8">
       <c r="C61"/>
       <c r="G61" s="10"/>
       <c r="H61" s="10"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8">
       <c r="G62" s="10"/>
       <c r="H62" s="12"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8">
       <c r="G63" s="10"/>
       <c r="H63" s="10"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8">
       <c r="G64" s="10"/>
       <c r="H64" s="10"/>
     </row>
-    <row r="65" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="7:8">
       <c r="G65" s="10"/>
       <c r="H65" s="10"/>
     </row>
-    <row r="66" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="7:8">
       <c r="G66" s="10"/>
       <c r="H66" s="10"/>
     </row>
-    <row r="67" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="7:8">
       <c r="G67" s="10"/>
       <c r="H67" s="10"/>
     </row>
-    <row r="68" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="7:8">
       <c r="G68" s="10"/>
       <c r="H68" s="10"/>
     </row>
-    <row r="69" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="7:8">
       <c r="G69" s="10"/>
       <c r="H69" s="10"/>
     </row>
-    <row r="70" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="7:8">
       <c r="G70" s="10"/>
       <c r="H70" s="10"/>
     </row>
-    <row r="71" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="7:8">
       <c r="G71" s="10"/>
       <c r="H71" s="10"/>
     </row>
-    <row r="72" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="7:8">
       <c r="G72" s="10"/>
       <c r="H72" s="10"/>
     </row>
-    <row r="73" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="7:8">
       <c r="G73" s="10"/>
       <c r="H73" s="10"/>
     </row>
-    <row r="74" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="7:8">
       <c r="G74" s="10"/>
       <c r="H74" s="10"/>
     </row>
-    <row r="75" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="7:8">
       <c r="G75" s="10"/>
       <c r="H75" s="10"/>
     </row>
-    <row r="76" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="7:8">
       <c r="G76" s="10"/>
       <c r="H76" s="10"/>
     </row>
-    <row r="77" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="7:8">
       <c r="G77" s="10"/>
       <c r="H77" s="10"/>
     </row>
-    <row r="78" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="7:8">
       <c r="G78" s="10"/>
       <c r="H78" s="10"/>
     </row>
-    <row r="79" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="7:8">
       <c r="G79" s="10"/>
       <c r="H79" s="10"/>
     </row>
-    <row r="80" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="7:8">
       <c r="G80" s="10"/>
       <c r="H80" s="10"/>
     </row>
-    <row r="81" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="7:8">
       <c r="G81" s="10"/>
       <c r="H81" s="10"/>
     </row>
-    <row r="82" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="7:8">
       <c r="G82" s="10"/>
       <c r="H82" s="10"/>
     </row>
-    <row r="83" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="7:8">
       <c r="G83" s="10"/>
       <c r="H83" s="11"/>
     </row>
-    <row r="84" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="7:8">
       <c r="G84" s="10"/>
       <c r="H84" s="10"/>
     </row>
-    <row r="85" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="7:8">
       <c r="G85" s="10"/>
       <c r="H85" s="10"/>
     </row>
-    <row r="86" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="7:8">
       <c r="G86" s="10"/>
       <c r="H86" s="10"/>
     </row>
-    <row r="87" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="7:8">
       <c r="G87" s="10"/>
       <c r="H87" s="10"/>
     </row>
-    <row r="88" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="7:8">
       <c r="G88" s="10"/>
       <c r="H88" s="10"/>
     </row>
@@ -3431,13 +3431,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.5703125" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1">
         <v>2017</v>
       </c>
@@ -3445,7 +3445,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="10" t="s">
         <v>88</v>
       </c>
@@ -3453,13 +3453,13 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="10" t="s">
         <v>89</v>
       </c>
       <c r="B3" s="10"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="10" t="s">
         <v>72</v>
       </c>
@@ -3467,7 +3467,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="10" t="s">
         <v>91</v>
       </c>
@@ -3475,7 +3475,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="10" t="s">
         <v>93</v>
       </c>
@@ -3483,7 +3483,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="10" t="s">
         <v>95</v>
       </c>
@@ -3491,7 +3491,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="10" t="s">
         <v>97</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" s="10" t="s">
         <v>98</v>
       </c>
@@ -3507,19 +3507,19 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" s="10"/>
       <c r="B10" s="10" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" s="10"/>
       <c r="B11" s="10" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" s="10" t="s">
         <v>70</v>
       </c>
@@ -3527,7 +3527,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" s="10" t="s">
         <v>74</v>
       </c>
@@ -3535,7 +3535,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" s="10" t="s">
         <v>102</v>
       </c>
@@ -3543,7 +3543,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" s="10" t="s">
         <v>103</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" s="10" t="s">
         <v>104</v>
       </c>
@@ -3559,7 +3559,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="10" t="s">
         <v>105</v>
       </c>
@@ -3567,7 +3567,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="10" t="s">
         <v>107</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="10" t="s">
         <v>108</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" s="10" t="s">
         <v>109</v>
       </c>
@@ -3591,7 +3591,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" s="10" t="s">
         <v>110</v>
       </c>
@@ -3599,7 +3599,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" s="10" t="s">
         <v>58</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" s="10" t="s">
         <v>113</v>
       </c>
@@ -3615,7 +3615,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" s="10" t="s">
         <v>115</v>
       </c>
@@ -3623,7 +3623,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" s="10" t="s">
         <v>117</v>
       </c>
@@ -3631,7 +3631,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" s="10" t="s">
         <v>119</v>
       </c>
@@ -3639,7 +3639,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27" s="10" t="s">
         <v>121</v>
       </c>
@@ -3647,7 +3647,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" s="10" t="s">
         <v>123</v>
       </c>
@@ -3655,13 +3655,13 @@
         <v>124</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" s="10" t="s">
         <v>125</v>
       </c>
       <c r="B29" s="10"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="A30" s="10" t="s">
         <v>60</v>
       </c>
@@ -3669,7 +3669,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="A31" s="10" t="s">
         <v>61</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32" s="10" t="s">
         <v>68</v>
       </c>
@@ -3685,7 +3685,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" s="10" t="s">
         <v>62</v>
       </c>
@@ -3693,7 +3693,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" s="10" t="s">
         <v>130</v>
       </c>
@@ -3701,7 +3701,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" s="10" t="s">
         <v>132</v>
       </c>
@@ -3709,7 +3709,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" s="10" t="s">
         <v>63</v>
       </c>
@@ -3717,7 +3717,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" s="10" t="s">
         <v>64</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38" s="10" t="s">
         <v>65</v>
       </c>
@@ -3733,7 +3733,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39" s="10" t="s">
         <v>66</v>
       </c>
@@ -3741,7 +3741,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40" s="10" t="s">
         <v>71</v>
       </c>
@@ -3749,7 +3749,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="A41" s="10" t="s">
         <v>67</v>
       </c>
@@ -3757,7 +3757,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42" s="10" t="s">
         <v>69</v>
       </c>
@@ -3765,7 +3765,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43" s="10" t="s">
         <v>141</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2">
       <c r="A44" s="10" t="s">
         <v>143</v>
       </c>
@@ -3781,7 +3781,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2">
       <c r="A45" s="10" t="s">
         <v>145</v>
       </c>
@@ -3789,7 +3789,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2">
       <c r="A46" s="10" t="s">
         <v>147</v>
       </c>
@@ -3797,7 +3797,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2">
       <c r="A47" s="10" t="s">
         <v>149</v>
       </c>
@@ -3805,7 +3805,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2">
       <c r="A48" s="10" t="s">
         <v>151</v>
       </c>
@@ -3813,7 +3813,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2">
       <c r="A49" s="10" t="s">
         <v>153</v>
       </c>
@@ -3821,7 +3821,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2">
       <c r="A50" s="10" t="s">
         <v>75</v>
       </c>
@@ -3829,7 +3829,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2">
       <c r="A51" s="10" t="s">
         <v>156</v>
       </c>
@@ -3837,7 +3837,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2">
       <c r="A52" s="10" t="s">
         <v>158</v>
       </c>
@@ -3845,7 +3845,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2">
       <c r="A53" s="13" t="s">
         <v>160</v>
       </c>
@@ -3853,7 +3853,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2">
       <c r="A54" s="13" t="s">
         <v>162</v>
       </c>
@@ -3861,13 +3861,13 @@
         <v>163</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2">
       <c r="A55" s="13" t="s">
         <v>164</v>
       </c>
       <c r="B55" s="10"/>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2">
       <c r="A56" s="13" t="s">
         <v>165</v>
       </c>
@@ -3875,13 +3875,13 @@
         <v>166</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2">
       <c r="A57" s="13" t="s">
         <v>167</v>
       </c>
       <c r="B57" s="10"/>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2">
       <c r="A58" s="13" t="s">
         <v>168</v>
       </c>
@@ -3889,7 +3889,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2">
       <c r="A59" s="13" t="s">
         <v>170</v>
       </c>
@@ -3897,7 +3897,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2">
       <c r="A60" s="13" t="s">
         <v>172</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2">
       <c r="A61" s="13" t="s">
         <v>174</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2">
       <c r="A62" s="13" t="s">
         <v>176</v>
       </c>
@@ -3921,13 +3921,13 @@
         <v>166</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2">
       <c r="A63" s="13" t="s">
         <v>177</v>
       </c>
       <c r="B63" s="10"/>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2">
       <c r="A64" s="13" t="s">
         <v>178</v>
       </c>
@@ -3935,7 +3935,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2">
       <c r="A65" s="13" t="s">
         <v>79</v>
       </c>
@@ -3943,7 +3943,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2">
       <c r="A66" s="13" t="s">
         <v>181</v>
       </c>
@@ -3951,7 +3951,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2">
       <c r="A67" s="13" t="s">
         <v>82</v>
       </c>
@@ -3959,13 +3959,13 @@
         <v>183</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2">
       <c r="A68" s="13"/>
       <c r="B68" s="10" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2">
       <c r="A69" s="13" t="s">
         <v>81</v>
       </c>
@@ -3973,13 +3973,13 @@
         <v>185</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2">
       <c r="A70" s="10"/>
       <c r="B70" s="10" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2">
       <c r="A71" s="10" t="s">
         <v>86</v>
       </c>
@@ -3987,7 +3987,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2">
       <c r="A72" s="10" t="s">
         <v>78</v>
       </c>
@@ -3995,13 +3995,13 @@
         <v>188</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2">
       <c r="A73" s="10" t="s">
         <v>77</v>
       </c>
       <c r="B73" s="10"/>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2">
       <c r="A74" s="10" t="s">
         <v>189</v>
       </c>
@@ -4009,7 +4009,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2">
       <c r="A75" s="10" t="s">
         <v>191</v>
       </c>
@@ -4017,13 +4017,13 @@
         <v>192</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2">
       <c r="A76" s="10" t="s">
         <v>193</v>
       </c>
       <c r="B76" s="10"/>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2">
       <c r="A77" s="10" t="s">
         <v>83</v>
       </c>
@@ -4031,7 +4031,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2">
       <c r="A78" s="10" t="s">
         <v>84</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2">
       <c r="A79" s="10" t="s">
         <v>196</v>
       </c>
@@ -4047,7 +4047,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2">
       <c r="A80" s="10" t="s">
         <v>85</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2">
       <c r="A81" s="10" t="s">
         <v>199</v>
       </c>
@@ -4063,13 +4063,13 @@
         <v>200</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2">
       <c r="A82" s="10"/>
       <c r="B82" s="11" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2">
       <c r="A83" s="10" t="s">
         <v>202</v>
       </c>
@@ -4077,7 +4077,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2">
       <c r="A84" s="10" t="s">
         <v>204</v>
       </c>
@@ -4085,7 +4085,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2">
       <c r="A85" s="10" t="s">
         <v>206</v>
       </c>
@@ -4093,7 +4093,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2">
       <c r="A86" s="10" t="s">
         <v>208</v>
       </c>
@@ -4101,7 +4101,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2">
       <c r="A87" s="10"/>
       <c r="B87" s="10" t="s">
         <v>210</v>
@@ -4116,18 +4116,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FD38E8-DCE1-4156-BA4C-4CE47C822C6C}">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="55" customWidth="1"/>
     <col min="2" max="2" width="47.140625" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="16" t="s">
         <v>251</v>
       </c>
@@ -4144,7 +4144,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="16.5">
       <c r="A2" t="s">
         <v>252</v>
       </c>
@@ -4158,7 +4158,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="16.5">
       <c r="A3" t="s">
         <v>253</v>
       </c>
@@ -4173,7 +4173,7 @@
       </c>
       <c r="E3" s="10"/>
     </row>
-    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="16.5">
       <c r="A4" t="s">
         <v>213</v>
       </c>
@@ -4188,7 +4188,7 @@
       </c>
       <c r="E4" s="10"/>
     </row>
-    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="16.5">
       <c r="A5" t="s">
         <v>254</v>
       </c>
@@ -4203,7 +4203,7 @@
       </c>
       <c r="E5" s="10"/>
     </row>
-    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="16.5">
       <c r="A6" t="s">
         <v>255</v>
       </c>
@@ -4218,7 +4218,7 @@
       </c>
       <c r="E6" s="10"/>
     </row>
-    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="16.5">
       <c r="A7" t="s">
         <v>256</v>
       </c>
@@ -4233,7 +4233,7 @@
       </c>
       <c r="E7" s="10"/>
     </row>
-    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="16.5">
       <c r="A8" t="s">
         <v>229</v>
       </c>
@@ -4247,7 +4247,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="16.5">
       <c r="A9" t="s">
         <v>230</v>
       </c>
@@ -4262,7 +4262,7 @@
       </c>
       <c r="E9" s="10"/>
     </row>
-    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="16.5">
       <c r="A10" t="s">
         <v>231</v>
       </c>
@@ -4277,7 +4277,7 @@
       </c>
       <c r="E10" s="10"/>
     </row>
-    <row r="11" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="16.5">
       <c r="A11" t="s">
         <v>232</v>
       </c>
@@ -4292,7 +4292,7 @@
       </c>
       <c r="E11" s="10"/>
     </row>
-    <row r="12" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="16.5">
       <c r="A12" t="s">
         <v>233</v>
       </c>
@@ -4307,7 +4307,7 @@
       </c>
       <c r="E12" s="10"/>
     </row>
-    <row r="13" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="16.5">
       <c r="A13" t="s">
         <v>234</v>
       </c>
@@ -4322,7 +4322,7 @@
       </c>
       <c r="E13" s="10"/>
     </row>
-    <row r="14" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="16.5">
       <c r="A14" t="s">
         <v>235</v>
       </c>
@@ -4337,7 +4337,7 @@
       </c>
       <c r="E14" s="10"/>
     </row>
-    <row r="15" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="16.5">
       <c r="A15" t="s">
         <v>257</v>
       </c>
@@ -4352,7 +4352,7 @@
       </c>
       <c r="E15" s="10"/>
     </row>
-    <row r="16" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="16.5">
       <c r="A16" t="s">
         <v>258</v>
       </c>
@@ -4366,7 +4366,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="16.5">
       <c r="A17" t="s">
         <v>259</v>
       </c>
@@ -4380,7 +4380,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="16.5">
       <c r="A18" t="s">
         <v>260</v>
       </c>
@@ -4394,7 +4394,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="16.5">
       <c r="A19" t="s">
         <v>261</v>
       </c>
@@ -4409,7 +4409,7 @@
       </c>
       <c r="E19" s="10"/>
     </row>
-    <row r="20" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="16.5">
       <c r="A20" t="s">
         <v>262</v>
       </c>
@@ -4424,7 +4424,7 @@
       </c>
       <c r="E20" s="14"/>
     </row>
-    <row r="21" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="16.5">
       <c r="A21" t="s">
         <v>238</v>
       </c>
@@ -4439,7 +4439,7 @@
       </c>
       <c r="E21" s="14"/>
     </row>
-    <row r="22" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="16.5">
       <c r="A22" t="s">
         <v>263</v>
       </c>
@@ -4454,7 +4454,7 @@
       </c>
       <c r="E22" s="14"/>
     </row>
-    <row r="23" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="16.5">
       <c r="A23" t="s">
         <v>239</v>
       </c>
@@ -4468,7 +4468,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="16.5">
       <c r="A24" t="s">
         <v>240</v>
       </c>
@@ -4482,7 +4482,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="16.5">
       <c r="A25" t="s">
         <v>241</v>
       </c>
@@ -4496,7 +4496,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="16.5">
       <c r="A26" t="s">
         <v>242</v>
       </c>
@@ -4511,7 +4511,7 @@
       </c>
       <c r="E26" s="10"/>
     </row>
-    <row r="27" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="16.5">
       <c r="A27" t="s">
         <v>243</v>
       </c>
@@ -4526,7 +4526,7 @@
       </c>
       <c r="E27" s="10"/>
     </row>
-    <row r="28" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="16.5">
       <c r="A28" t="s">
         <v>244</v>
       </c>
@@ -4540,7 +4540,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="16.5">
       <c r="A29" t="s">
         <v>245</v>
       </c>
@@ -4554,7 +4554,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="16.5">
       <c r="A30" t="s">
         <v>246</v>
       </c>
@@ -4568,7 +4568,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="16.5">
       <c r="A31" t="s">
         <v>247</v>
       </c>
@@ -4582,7 +4582,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="17.25">
       <c r="A32" t="s">
         <v>248</v>
       </c>
@@ -4596,7 +4596,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="16.5">
       <c r="A33" t="s">
         <v>264</v>
       </c>
@@ -4610,7 +4610,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="16.5">
       <c r="A34" t="s">
         <v>265</v>
       </c>
@@ -4625,7 +4625,7 @@
       </c>
       <c r="E34" s="10"/>
     </row>
-    <row r="35" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="16.5">
       <c r="A35" t="s">
         <v>266</v>
       </c>
@@ -4640,7 +4640,7 @@
       </c>
       <c r="E35" s="10"/>
     </row>
-    <row r="36" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="16.5">
       <c r="A36" t="s">
         <v>267</v>
       </c>
@@ -4655,7 +4655,7 @@
       </c>
       <c r="E36" s="10"/>
     </row>
-    <row r="37" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="16.5">
       <c r="A37" t="s">
         <v>249</v>
       </c>
@@ -4670,7 +4670,7 @@
       </c>
       <c r="E37" s="10"/>
     </row>
-    <row r="38" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="16.5">
       <c r="A38" t="s">
         <v>268</v>
       </c>
@@ -4685,7 +4685,7 @@
       </c>
       <c r="E38" s="14"/>
     </row>
-    <row r="39" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="16.5">
       <c r="A39" t="s">
         <v>269</v>
       </c>
@@ -4700,7 +4700,7 @@
       </c>
       <c r="E39" s="10"/>
     </row>
-    <row r="40" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="16.5">
       <c r="A40" t="s">
         <v>270</v>
       </c>
@@ -4714,7 +4714,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="16.5">
       <c r="A41" t="s">
         <v>271</v>
       </c>
@@ -4729,7 +4729,7 @@
       </c>
       <c r="E41" s="14"/>
     </row>
-    <row r="42" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="16.5">
       <c r="A42" t="s">
         <v>272</v>
       </c>
@@ -4744,7 +4744,7 @@
       </c>
       <c r="E42" s="10"/>
     </row>
-    <row r="43" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="16.5">
       <c r="A43" t="s">
         <v>250</v>
       </c>
@@ -4758,7 +4758,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="16.5">
       <c r="A44" t="s">
         <v>214</v>
       </c>
@@ -4772,7 +4772,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="16.5">
       <c r="A45" t="s">
         <v>215</v>
       </c>
@@ -4786,7 +4786,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="16.5">
       <c r="A46" t="s">
         <v>216</v>
       </c>
@@ -4800,7 +4800,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="16.5">
       <c r="A47" t="s">
         <v>217</v>
       </c>
@@ -4814,7 +4814,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="16.5">
       <c r="A48" t="s">
         <v>218</v>
       </c>
@@ -4828,7 +4828,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="16.5">
       <c r="A49" t="s">
         <v>219</v>
       </c>
@@ -4842,7 +4842,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="16.5">
       <c r="A50" s="15" t="s">
         <v>220</v>
       </c>
@@ -4859,7 +4859,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="16.5">
       <c r="A51" t="s">
         <v>273</v>
       </c>
@@ -4873,7 +4873,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="16.5">
       <c r="A52" t="s">
         <v>221</v>
       </c>
@@ -4888,7 +4888,7 @@
       </c>
       <c r="E52" s="10"/>
     </row>
-    <row r="53" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="16.5">
       <c r="A53" t="s">
         <v>274</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" ht="16.5">
       <c r="A54" t="s">
         <v>275</v>
       </c>
@@ -4916,7 +4916,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" ht="16.5">
       <c r="A55" t="s">
         <v>276</v>
       </c>
@@ -4930,7 +4930,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" ht="16.5">
       <c r="A56" t="s">
         <v>222</v>
       </c>
@@ -4944,7 +4944,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" ht="33">
       <c r="A57" t="s">
         <v>223</v>
       </c>
@@ -4958,7 +4958,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="16.5">
       <c r="A58" t="s">
         <v>277</v>
       </c>
@@ -4972,7 +4972,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" ht="16.5">
       <c r="A59" t="s">
         <v>278</v>
       </c>
@@ -4986,7 +4986,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" ht="16.5">
       <c r="A60" s="15" t="s">
         <v>224</v>
       </c>
@@ -5003,7 +5003,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" ht="16.5">
       <c r="A61" t="s">
         <v>279</v>
       </c>
@@ -5017,7 +5017,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" ht="16.5">
       <c r="A62" t="s">
         <v>225</v>
       </c>
@@ -5031,7 +5031,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" ht="16.5">
       <c r="A63" t="s">
         <v>226</v>
       </c>
@@ -5045,7 +5045,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" ht="16.5">
       <c r="A64" t="s">
         <v>227</v>
       </c>
@@ -5059,7 +5059,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" ht="16.5">
       <c r="A65" t="s">
         <v>228</v>
       </c>
@@ -5073,7 +5073,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" ht="16.5">
       <c r="A66" t="s">
         <v>236</v>
       </c>
@@ -5087,7 +5087,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" ht="16.5">
       <c r="A67" t="s">
         <v>237</v>
       </c>
@@ -5101,7 +5101,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" ht="16.5">
       <c r="C68" s="1" t="s">
         <v>2</v>
       </c>
@@ -5109,7 +5109,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" ht="16.5">
       <c r="C69" s="1" t="s">
         <v>41</v>
       </c>
@@ -5117,7 +5117,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" ht="16.5">
       <c r="C70" s="1" t="s">
         <v>51</v>
       </c>
@@ -5125,7 +5125,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" ht="16.5">
       <c r="C71" s="1" t="s">
         <v>52</v>
       </c>
@@ -5143,17 +5143,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05164C71-A70B-4BC7-B5B5-94FB28BB5C0F}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.140625" customWidth="1"/>
     <col min="2" max="2" width="40.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="16" t="s">
         <v>302</v>
       </c>
@@ -5167,7 +5167,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="16.5">
       <c r="A2" s="18" t="s">
         <v>194</v>
       </c>
@@ -5178,7 +5178,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="16.5">
       <c r="A3" s="18" t="s">
         <v>197</v>
       </c>
@@ -5192,7 +5192,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="16.5">
       <c r="A4" s="18" t="s">
         <v>201</v>
       </c>
@@ -5203,7 +5203,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="16.5">
       <c r="A5" s="18" t="s">
         <v>127</v>
       </c>
@@ -5214,7 +5214,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="16.5">
       <c r="A6" s="18" t="s">
         <v>129</v>
       </c>
@@ -5224,7 +5224,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="16.5">
       <c r="A7" s="18" t="s">
         <v>203</v>
       </c>
@@ -5235,7 +5235,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="16.5">
       <c r="A8" s="18" t="s">
         <v>155</v>
       </c>
@@ -5246,7 +5246,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="16.5">
       <c r="A9" s="18" t="s">
         <v>195</v>
       </c>
@@ -5257,7 +5257,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="16.5">
       <c r="A10" s="18" t="s">
         <v>135</v>
       </c>
@@ -5268,7 +5268,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="16.5">
       <c r="A11" s="18" t="s">
         <v>126</v>
       </c>
@@ -5279,7 +5279,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="16.5">
       <c r="A12" s="18" t="s">
         <v>137</v>
       </c>
@@ -5290,7 +5290,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="16.5">
       <c r="A13" s="18" t="s">
         <v>134</v>
       </c>
@@ -5301,7 +5301,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="16.5">
       <c r="A14" s="18" t="s">
         <v>136</v>
       </c>
@@ -5312,7 +5312,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="16.5">
       <c r="A15" s="18" t="s">
         <v>140</v>
       </c>
@@ -5323,7 +5323,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="18" t="s">
         <v>70</v>
       </c>
@@ -5343,17 +5343,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FAB965F-4D5B-450A-BC9E-4BCCD940211B}">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="55" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="16" t="s">
         <v>307</v>
       </c>
@@ -5367,7 +5367,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="16.5">
       <c r="B2" t="s">
         <v>252</v>
       </c>
@@ -5378,7 +5378,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="16.5">
       <c r="B3" t="s">
         <v>253</v>
       </c>
@@ -5389,7 +5389,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="16.5">
       <c r="B4" t="s">
         <v>213</v>
       </c>
@@ -5400,7 +5400,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="16.5">
       <c r="B5" t="s">
         <v>254</v>
       </c>
@@ -5411,7 +5411,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="16.5">
       <c r="B6" t="s">
         <v>255</v>
       </c>
@@ -5422,7 +5422,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="16.5">
       <c r="B7" t="s">
         <v>256</v>
       </c>
@@ -5433,7 +5433,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="16.5">
       <c r="B8" t="s">
         <v>229</v>
       </c>
@@ -5444,7 +5444,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="16.5">
       <c r="B9" t="s">
         <v>230</v>
       </c>
@@ -5455,7 +5455,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="16.5">
       <c r="B10" t="s">
         <v>231</v>
       </c>
@@ -5466,7 +5466,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="16.5">
       <c r="B11" t="s">
         <v>232</v>
       </c>
@@ -5477,7 +5477,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="16.5">
       <c r="B12" t="s">
         <v>233</v>
       </c>
@@ -5488,7 +5488,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="16.5">
       <c r="B13" t="s">
         <v>234</v>
       </c>
@@ -5499,7 +5499,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="16.5">
       <c r="B14" t="s">
         <v>235</v>
       </c>
@@ -5510,7 +5510,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="16.5">
       <c r="B15" t="s">
         <v>257</v>
       </c>
@@ -5521,7 +5521,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="16.5">
       <c r="B16" t="s">
         <v>258</v>
       </c>
@@ -5532,7 +5532,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" ht="16.5">
       <c r="B17" t="s">
         <v>259</v>
       </c>
@@ -5543,7 +5543,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" ht="16.5">
       <c r="B18" t="s">
         <v>260</v>
       </c>
@@ -5554,7 +5554,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" ht="16.5">
       <c r="B19" t="s">
         <v>261</v>
       </c>
@@ -5565,7 +5565,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" ht="16.5">
       <c r="B20" t="s">
         <v>262</v>
       </c>
@@ -5576,7 +5576,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" ht="16.5">
       <c r="B21" t="s">
         <v>238</v>
       </c>
@@ -5587,7 +5587,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" ht="16.5">
       <c r="B22" t="s">
         <v>263</v>
       </c>
@@ -5598,7 +5598,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" ht="16.5">
       <c r="B23" t="s">
         <v>239</v>
       </c>
@@ -5609,7 +5609,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4" ht="16.5">
       <c r="B24" t="s">
         <v>240</v>
       </c>
@@ -5620,7 +5620,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" ht="16.5">
       <c r="B25" t="s">
         <v>241</v>
       </c>
@@ -5631,7 +5631,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:4" ht="16.5">
       <c r="B26" t="s">
         <v>242</v>
       </c>
@@ -5642,7 +5642,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:4" ht="16.5">
       <c r="B27" t="s">
         <v>243</v>
       </c>
@@ -5653,7 +5653,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:4" ht="16.5">
       <c r="B28" t="s">
         <v>244</v>
       </c>
@@ -5664,7 +5664,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:4" ht="16.5">
       <c r="B29" t="s">
         <v>245</v>
       </c>
@@ -5675,7 +5675,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:4" ht="16.5">
       <c r="B30" t="s">
         <v>246</v>
       </c>
@@ -5686,7 +5686,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:4" ht="16.5">
       <c r="B31" t="s">
         <v>247</v>
       </c>
@@ -5697,7 +5697,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:4" ht="17.25">
       <c r="B32" t="s">
         <v>248</v>
       </c>
@@ -5708,7 +5708,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" ht="16.5">
       <c r="B33" t="s">
         <v>264</v>
       </c>
@@ -5719,7 +5719,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" ht="16.5">
       <c r="B34" t="s">
         <v>265</v>
       </c>
@@ -5730,7 +5730,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" ht="16.5">
       <c r="B35" t="s">
         <v>266</v>
       </c>
@@ -5741,7 +5741,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" ht="16.5">
       <c r="B36" t="s">
         <v>267</v>
       </c>
@@ -5752,7 +5752,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" ht="16.5">
       <c r="B37" t="s">
         <v>249</v>
       </c>
@@ -5763,7 +5763,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" ht="16.5">
       <c r="B38" t="s">
         <v>268</v>
       </c>
@@ -5774,7 +5774,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" ht="16.5">
       <c r="B39" t="s">
         <v>269</v>
       </c>
@@ -5785,7 +5785,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" ht="16.5">
       <c r="B40" t="s">
         <v>270</v>
       </c>
@@ -5796,7 +5796,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" ht="16.5">
       <c r="B41" t="s">
         <v>271</v>
       </c>
@@ -5807,7 +5807,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" ht="16.5">
       <c r="B42" t="s">
         <v>272</v>
       </c>
@@ -5818,7 +5818,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4" ht="16.5">
       <c r="B43" t="s">
         <v>250</v>
       </c>
@@ -5829,7 +5829,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="44" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:4" ht="16.5">
       <c r="B44" t="s">
         <v>214</v>
       </c>
@@ -5840,7 +5840,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="45" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:4" ht="16.5">
       <c r="B45" t="s">
         <v>215</v>
       </c>
@@ -5851,7 +5851,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="46" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:4" ht="16.5">
       <c r="B46" t="s">
         <v>216</v>
       </c>
@@ -5862,7 +5862,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="47" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:4" ht="16.5">
       <c r="B47" t="s">
         <v>217</v>
       </c>
@@ -5873,7 +5873,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="48" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:4" ht="16.5">
       <c r="B48" t="s">
         <v>218</v>
       </c>
@@ -5884,7 +5884,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="49" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:4" ht="16.5">
       <c r="B49" t="s">
         <v>219</v>
       </c>
@@ -5895,7 +5895,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="50" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:4" ht="16.5">
       <c r="B50" s="15" t="s">
         <v>220</v>
       </c>
@@ -5906,7 +5906,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:4" ht="16.5">
       <c r="B51" t="s">
         <v>273</v>
       </c>
@@ -5917,7 +5917,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="52" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:4" ht="16.5">
       <c r="B52" t="s">
         <v>221</v>
       </c>
@@ -5928,7 +5928,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="53" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:4" ht="16.5">
       <c r="B53" t="s">
         <v>274</v>
       </c>
@@ -5939,7 +5939,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="54" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:4" ht="16.5">
       <c r="B54" t="s">
         <v>275</v>
       </c>
@@ -5950,7 +5950,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:4" ht="16.5">
       <c r="B55" t="s">
         <v>276</v>
       </c>
@@ -5961,7 +5961,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:4" ht="16.5">
       <c r="B56" t="s">
         <v>222</v>
       </c>
@@ -5972,7 +5972,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="57" spans="2:4" ht="33" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:4" ht="33">
       <c r="B57" t="s">
         <v>223</v>
       </c>
@@ -5983,7 +5983,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:4" ht="16.5">
       <c r="B58" t="s">
         <v>277</v>
       </c>
@@ -5994,7 +5994,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="59" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:4" ht="16.5">
       <c r="B59" t="s">
         <v>278</v>
       </c>
@@ -6005,7 +6005,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="60" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:4" ht="16.5">
       <c r="B60" s="15" t="s">
         <v>224</v>
       </c>
@@ -6016,7 +6016,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="61" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:4" ht="16.5">
       <c r="B61" t="s">
         <v>279</v>
       </c>
@@ -6027,7 +6027,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="62" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:4" ht="16.5">
       <c r="B62" t="s">
         <v>225</v>
       </c>
@@ -6038,7 +6038,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="63" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:4" ht="16.5">
       <c r="B63" t="s">
         <v>226</v>
       </c>
@@ -6049,7 +6049,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="64" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:4" ht="16.5">
       <c r="B64" t="s">
         <v>227</v>
       </c>
@@ -6060,7 +6060,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="65" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:4" ht="16.5">
       <c r="B65" t="s">
         <v>228</v>
       </c>
@@ -6071,7 +6071,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="66" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:4" ht="16.5">
       <c r="B66" t="s">
         <v>236</v>
       </c>
@@ -6082,7 +6082,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="67" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:4" ht="16.5">
       <c r="B67" t="s">
         <v>237</v>
       </c>
@@ -6093,7 +6093,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="68" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:4" ht="16.5">
       <c r="C68" s="1" t="s">
         <v>2</v>
       </c>
@@ -6101,7 +6101,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="69" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:4" ht="16.5">
       <c r="C69" s="1" t="s">
         <v>41</v>
       </c>
@@ -6109,7 +6109,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="70" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:4" ht="16.5">
       <c r="C70" s="1" t="s">
         <v>51</v>
       </c>
@@ -6117,7 +6117,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="71" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:4" ht="16.5">
       <c r="C71" s="1" t="s">
         <v>52</v>
       </c>
@@ -6143,9 +6143,9 @@
       <selection activeCell="AD24" sqref="AD24:AE24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="16" t="s">
         <v>286</v>
       </c>
@@ -6159,7 +6159,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>292</v>
       </c>
@@ -6170,7 +6170,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>293</v>
       </c>
@@ -6181,7 +6181,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>294</v>
       </c>
@@ -6192,7 +6192,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>295</v>
       </c>

</xml_diff>